<commit_message>
Support MXR oscilloscope's csv data formart
</commit_message>
<xml_diff>
--- a/Converter/assets/UnitConversion.xlsx
+++ b/Converter/assets/UnitConversion.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d78e2062db64e14/Project/Python/AnalysisTool/Converter/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://photonicinc-my.sharepoint.com/personal/iyoneda_photonic_com/Documents/Python/AnalysisTool/Converter/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="405" documentId="13_ncr:1_{4CCCEAE6-5D0C-4A8E-AD1B-C17E928355D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1ECE3C1-9189-419B-8F2B-1A393B83A904}"/>
+  <xr:revisionPtr revIDLastSave="434" documentId="13_ncr:1_{4CCCEAE6-5D0C-4A8E-AD1B-C17E928355D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{018A6435-C738-46EF-A3CC-00981DD05CAB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1695" windowWidth="9945" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6942" yWindow="696" windowWidth="13938" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elec" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elec!$A$1:$Q$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elec!$A$1:$Q$123</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="398">
   <si>
     <t>No</t>
   </si>
@@ -1193,6 +1193,30 @@
   </si>
   <si>
     <t>DegreesF</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>[MHz]</t>
+  </si>
+  <si>
+    <t>[Point]</t>
+  </si>
+  <si>
+    <t>MHz GSAperSec</t>
+  </si>
+  <si>
+    <t>"r'$Datapoints[Point] = \frac{Sampling Frequency[GSa/s] \times 10^9}{Frequency [MHz] \times 10^6}$'"</t>
+  </si>
+  <si>
+    <t>(P[1] * sympy.Pow(10,9))/(P[0]* sympy.Pow(10,6))</t>
+  </si>
+  <si>
+    <t>DataRate [MHz]</t>
+  </si>
+  <si>
+    <t>SamplingPoints [Gsa/s]</t>
   </si>
 </sst>
 </file>
@@ -1608,33 +1632,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:Q123"/>
+  <dimension ref="A1:Q124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M129" sqref="M129"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.05078125" defaultRowHeight="18.3" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="9.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.20703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="89.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="102.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="14.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.06640625" style="5"/>
+    <col min="9" max="9" width="89.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="102.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.26171875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.05078125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +1711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1730,7 +1754,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1771,7 +1795,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1809,7 +1833,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1847,7 +1871,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1885,7 +1909,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1923,7 +1947,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1961,7 +1985,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1999,7 +2023,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2037,7 +2061,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2075,7 +2099,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2116,7 +2140,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2157,7 +2181,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2203,7 +2227,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2241,7 +2265,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2282,7 +2306,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2320,7 +2344,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2358,7 +2382,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2396,7 +2420,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2434,7 +2458,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2472,7 +2496,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2507,7 +2531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2542,7 +2566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2580,7 +2604,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2618,7 +2642,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2653,7 +2677,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2694,7 +2718,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2732,7 +2756,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2770,7 +2794,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2808,7 +2832,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2846,7 +2870,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2884,7 +2908,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2919,7 +2943,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2957,7 +2981,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2998,7 +3022,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3036,7 +3060,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3077,7 +3101,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3118,7 +3142,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3159,7 +3183,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3197,7 +3221,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3235,7 +3259,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3276,7 +3300,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3314,7 +3338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3349,7 +3373,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3384,7 +3408,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3422,7 +3446,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3460,7 +3484,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.7">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3498,7 +3522,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3536,7 +3560,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3574,7 +3598,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3612,7 +3636,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3650,7 +3674,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3688,7 +3712,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3729,7 +3753,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3770,7 +3794,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3811,7 +3835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3852,7 +3876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3893,7 +3917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3934,7 +3958,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3972,7 +3996,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4013,7 +4037,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4057,7 +4081,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4098,7 +4122,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4136,7 +4160,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4177,7 +4201,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4218,7 +4242,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4262,7 +4286,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4297,7 +4321,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4335,7 +4359,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4373,7 +4397,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4411,7 +4435,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4449,7 +4473,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4487,7 +4511,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4525,7 +4549,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4560,7 +4584,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4601,7 +4625,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -4642,7 +4666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -4683,7 +4707,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -4721,7 +4745,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -4756,7 +4780,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4800,7 +4824,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -4838,7 +4862,7 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
     </row>
-    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4881,7 +4905,7 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4919,7 +4943,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4957,7 +4981,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -4992,7 +5016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5027,7 +5051,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5062,7 +5086,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5097,7 +5121,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.7">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5132,7 +5156,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
       <c r="B91" s="1" t="s">
         <v>286</v>
       </c>
@@ -5164,7 +5191,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
       <c r="B92" s="1" t="s">
         <v>286</v>
       </c>
@@ -5196,7 +5226,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
       <c r="B93" s="1" t="s">
         <v>286</v>
       </c>
@@ -5228,7 +5261,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
       <c r="B94" s="1" t="s">
         <v>286</v>
       </c>
@@ -5260,7 +5296,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
       <c r="B95" s="1" t="s">
         <v>286</v>
       </c>
@@ -5292,7 +5331,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
       <c r="B96" s="1" t="s">
         <v>286</v>
       </c>
@@ -5324,7 +5366,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="97" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
       <c r="B97" s="1" t="s">
         <v>286</v>
       </c>
@@ -5356,7 +5401,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="98" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
       <c r="B98" s="1" t="s">
         <v>286</v>
       </c>
@@ -5388,7 +5436,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="99" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
       <c r="B99" s="1" t="s">
         <v>286</v>
       </c>
@@ -5420,7 +5471,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="100" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
       <c r="B100" s="1" t="s">
         <v>286</v>
       </c>
@@ -5452,7 +5506,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="101" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
       <c r="B101" s="1" t="s">
         <v>286</v>
       </c>
@@ -5484,7 +5541,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="102" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
       <c r="B102" s="1" t="s">
         <v>286</v>
       </c>
@@ -5516,7 +5576,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="103" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
       <c r="B103" s="1" t="s">
         <v>286</v>
       </c>
@@ -5548,7 +5611,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="104" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
       <c r="B104" s="1" t="s">
         <v>286</v>
       </c>
@@ -5580,7 +5646,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="105" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
       <c r="B105" s="1" t="s">
         <v>286</v>
       </c>
@@ -5612,7 +5681,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="106" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
       <c r="B106" s="1" t="s">
         <v>286</v>
       </c>
@@ -5644,7 +5716,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="107" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
       <c r="B107" s="1" t="s">
         <v>286</v>
       </c>
@@ -5676,7 +5751,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="108" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
       <c r="B108" s="1" t="s">
         <v>286</v>
       </c>
@@ -5708,7 +5786,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="109" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
       <c r="B109" s="1" t="s">
         <v>286</v>
       </c>
@@ -5740,7 +5821,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="110" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
       <c r="B110" s="1" t="s">
         <v>286</v>
       </c>
@@ -5772,7 +5856,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="111" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
       <c r="B111" s="1" t="s">
         <v>286</v>
       </c>
@@ -5804,7 +5891,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="112" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
       <c r="B112" s="1" t="s">
         <v>286</v>
       </c>
@@ -5836,7 +5926,10 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="113" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
       <c r="B113" s="1" t="s">
         <v>286</v>
       </c>
@@ -5868,7 +5961,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
       <c r="B114" s="1" t="s">
         <v>286</v>
       </c>
@@ -5900,7 +5996,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
       <c r="B115" s="1" t="s">
         <v>286</v>
       </c>
@@ -5932,7 +6031,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
       <c r="B116" s="1" t="s">
         <v>286</v>
       </c>
@@ -5964,7 +6066,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
       <c r="B117" s="1" t="s">
         <v>286</v>
       </c>
@@ -5996,7 +6101,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
       <c r="B118" s="1" t="s">
         <v>286</v>
       </c>
@@ -6028,7 +6136,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="2:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
       <c r="B119" s="1" t="s">
         <v>286</v>
       </c>
@@ -6060,7 +6171,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A120" s="1">
+        <v>119</v>
+      </c>
       <c r="B120" s="1" t="s">
         <v>32</v>
       </c>
@@ -6095,7 +6209,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A121" s="1">
+        <v>120</v>
+      </c>
       <c r="B121" s="1" t="s">
         <v>32</v>
       </c>
@@ -6130,7 +6247,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
       <c r="B122" s="1" t="s">
         <v>379</v>
       </c>
@@ -6162,7 +6282,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A123" s="1">
+        <v>122</v>
+      </c>
       <c r="B123" s="1" t="s">
         <v>379</v>
       </c>
@@ -6194,13 +6317,49 @@
         <v>100</v>
       </c>
     </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.7">
+      <c r="A124" s="1">
+        <v>123</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="L124" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M124" s="1">
+        <v>100</v>
+      </c>
+      <c r="N124" s="1">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q119" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="MECH"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:Q123" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q85">
       <sortCondition ref="C1:C85"/>
     </sortState>

</xml_diff>

<commit_message>
Adding Vavg and Vpp
</commit_message>
<xml_diff>
--- a/Converter/assets/UnitConversion.xlsx
+++ b/Converter/assets/UnitConversion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://photonicinc-my.sharepoint.com/personal/iyoneda_photonic_com/Documents/Python/AnalysisTool/Converter/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d78e2062db64e14/Project/Python/AnalysisTool/Converter/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="434" documentId="13_ncr:1_{4CCCEAE6-5D0C-4A8E-AD1B-C17E928355D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{018A6435-C738-46EF-A3CC-00981DD05CAB}"/>
+  <xr:revisionPtr revIDLastSave="505" documentId="13_ncr:1_{4CCCEAE6-5D0C-4A8E-AD1B-C17E928355D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7259BB6-1205-4D2E-877F-0C72133AB6AF}"/>
   <bookViews>
-    <workbookView xWindow="6942" yWindow="696" windowWidth="13938" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1695" windowWidth="9113" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elec" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="419">
   <si>
     <t>No</t>
   </si>
@@ -1217,6 +1217,69 @@
   </si>
   <si>
     <t>SamplingPoints [Gsa/s]</t>
+  </si>
+  <si>
+    <t>Voltage [Vp]</t>
+  </si>
+  <si>
+    <t>[Vp]</t>
+  </si>
+  <si>
+    <t>sympy.Pow(2,0.5) * P[0]</t>
+  </si>
+  <si>
+    <t>"r'$Voltage [Vpeak] = \sqrt{2} \times Voltage[V]$'"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P[0]/sympy.Pow(2,0.5)</t>
+  </si>
+  <si>
+    <t>"r'$Voltage [V] = \frac{Voltage[Vpeak]}{\sqrt{2}}$'"</t>
+  </si>
+  <si>
+    <t>Voltage [Vpp]</t>
+  </si>
+  <si>
+    <t>[Vpp]</t>
+  </si>
+  <si>
+    <t>2*sympy.Pow(2,0.5) * P[0]</t>
+  </si>
+  <si>
+    <t>"r'$Voltage [Vpeak-peak] =2 \sqrt{2} \times Voltage[V]$'"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P[0]/(2*sympy.Pow(2,0.5))</t>
+  </si>
+  <si>
+    <t>Voltage [Vavg]</t>
+  </si>
+  <si>
+    <t>[Vavg]</t>
+  </si>
+  <si>
+    <t>sympy.pi*P[0]/(2*sympy.Pow(2,0.5))</t>
+  </si>
+  <si>
+    <t>"r'$Voltage [V] = \frac{\pi \times Voltage[Vavg]}{2\sqrt{2}}$'"</t>
+  </si>
+  <si>
+    <t>Vp</t>
+  </si>
+  <si>
+    <t>Vpp</t>
+  </si>
+  <si>
+    <t>"r'$Voltage [V] = \frac{Voltage[Vpeak-peak]}{2\sqrt{2}}$'"</t>
+  </si>
+  <si>
+    <t>Vavg</t>
+  </si>
+  <si>
+    <t>"r'$Voltage [Vavg] = \frac{2\sqrt{2}}{\pi} \times Voltage [V]$'"</t>
+  </si>
+  <si>
+    <t>(2*sympy.Pow(2,0.5)*P[0])/sympy.pi</t>
   </si>
 </sst>
 </file>
@@ -1632,33 +1695,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q124"/>
+  <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E125" sqref="E125"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I136" sqref="I136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.05078125" defaultRowHeight="18.3" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="89.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="102.5234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.20703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="14.26171875" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.05078125" style="5"/>
+    <col min="9" max="9" width="89.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="102.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.06640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1711,7 +1774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1754,7 +1817,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1795,7 +1858,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1833,7 +1896,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1871,7 +1934,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1909,7 +1972,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1947,7 +2010,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1985,7 +2048,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2023,7 +2086,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2061,7 +2124,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2099,7 +2162,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2140,7 +2203,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2181,7 +2244,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2227,7 +2290,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2265,7 +2328,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2306,7 +2369,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2344,7 +2407,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2382,7 +2445,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2420,7 +2483,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2458,7 +2521,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2496,7 +2559,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2531,7 +2594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2566,7 +2629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2604,7 +2667,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2642,7 +2705,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2677,7 +2740,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2718,7 +2781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2756,7 +2819,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2794,7 +2857,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2832,7 +2895,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2870,7 +2933,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2908,7 +2971,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2943,7 +3006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2981,7 +3044,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3022,7 +3085,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3060,7 +3123,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3101,7 +3164,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3142,7 +3205,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3183,7 +3246,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3221,7 +3284,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3259,7 +3322,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3300,7 +3363,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3338,7 +3401,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3373,7 +3436,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3408,7 +3471,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3446,7 +3509,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3484,7 +3547,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3522,7 +3585,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3560,7 +3623,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3598,7 +3661,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3636,7 +3699,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3674,7 +3737,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3712,7 +3775,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3753,7 +3816,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3794,7 +3857,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3835,7 +3898,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3876,7 +3939,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3917,7 +3980,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3958,7 +4021,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3996,7 +4059,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4037,7 +4100,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4081,7 +4144,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4122,7 +4185,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4160,7 +4223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4201,7 +4264,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4242,7 +4305,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4286,7 +4349,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4321,7 +4384,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4359,7 +4422,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4397,7 +4460,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4435,7 +4498,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4473,7 +4536,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4511,7 +4574,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4549,7 +4612,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4584,7 +4647,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4625,7 +4688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -4666,7 +4729,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -4707,7 +4770,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -4745,7 +4808,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -4780,7 +4843,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4824,7 +4887,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -4862,7 +4925,7 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4905,7 +4968,7 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4943,7 +5006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4981,7 +5044,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5016,7 +5079,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5051,7 +5114,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5086,7 +5149,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5121,7 +5184,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5156,7 +5219,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5191,7 +5254,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5226,7 +5289,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5261,7 +5324,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5296,7 +5359,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5331,7 +5394,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5366,7 +5429,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -5401,7 +5464,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -5436,7 +5499,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -5471,7 +5534,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -5506,7 +5569,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -5541,7 +5604,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -5576,7 +5639,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -5611,7 +5674,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -5646,7 +5709,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -5681,7 +5744,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -5716,7 +5779,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -5751,7 +5814,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -5786,7 +5849,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -5821,7 +5884,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -5856,7 +5919,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -5891,7 +5954,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -5926,7 +5989,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -5961,7 +6024,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -5996,7 +6059,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -6031,7 +6094,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -6066,7 +6129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -6101,7 +6164,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -6136,7 +6199,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -6171,7 +6234,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -6209,7 +6272,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -6247,7 +6310,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -6282,7 +6345,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -6317,7 +6380,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.7">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -6356,6 +6419,216 @@
       </c>
       <c r="N124" s="1">
         <v>64</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="1">
+        <v>124</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L125" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M125" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="1">
+        <v>125</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="L126" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M126" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L127" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M127" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="1">
+        <v>125</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="J128" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="L128" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M128" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="1">
+        <v>125</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="L129" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M129" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="1">
+        <v>125</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="J130" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L130" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M130" s="1">
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Aborsption loss formula
</commit_message>
<xml_diff>
--- a/Converter/assets/UnitConversion.xlsx
+++ b/Converter/assets/UnitConversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d78e2062db64e14/Project/Python/AnalysisTool/Converter/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="505" documentId="13_ncr:1_{4CCCEAE6-5D0C-4A8E-AD1B-C17E928355D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7259BB6-1205-4D2E-877F-0C72133AB6AF}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{28AA09F0-1BFD-4629-8D14-FBC6BDF866C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{035093EF-A928-4F0C-9420-79F400ECAB0C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1695" windowWidth="9113" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="14550" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elec" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="441">
   <si>
     <t>No</t>
   </si>
@@ -1280,6 +1280,72 @@
   </si>
   <si>
     <t>(2*sympy.Pow(2,0.5)*P[0])/sympy.pi</t>
+  </si>
+  <si>
+    <t>Frequency [Hz]</t>
+  </si>
+  <si>
+    <t>[Hz]</t>
+  </si>
+  <si>
+    <t>Skin-Depth (Cu) [m]</t>
+  </si>
+  <si>
+    <t>sympy.Pow((2)/(2*sympy.pi*P[0]*P[1]*P[2]),0.5)</t>
+  </si>
+  <si>
+    <t>Skin-Depth (Al) [m]</t>
+  </si>
+  <si>
+    <t>"r'$SkinDepth (Cu)[m] = \sqrt{\frac{2}{2\pi Frequency[Hz] \times Permetivity {\mu} [H/m] \times Conductibity \sigma[S/m]}}$'"</t>
+  </si>
+  <si>
+    <t>"r'$SkinDepth (Al)[m] = \sqrt{\frac{2}{2\pi Frequency[Hz] \times Permetivity {\mu} [H/m] \times Conductibity \sigma[S/m]}}$'"</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Cu Conductivity:Cu</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Al Conductivity:Al</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Fe Conductivity:Fe</t>
+  </si>
+  <si>
+    <t>"r'$SkinDepth (Fe)[m] = \sqrt{\frac{2}{2\pi Frequency[Hz] \times Permetivity {\mu} [H/m] \times Conductibity \sigma[S/m]}}$'"</t>
+  </si>
+  <si>
+    <t>Skin-Depth (Fe) [m]</t>
+  </si>
+  <si>
+    <t>Abosrption Loss (Cu) [dB]</t>
+  </si>
+  <si>
+    <t>"r'$Absorption Loss (Cu) [dB] = 8.69 \times \frac{Sheild Thickness [mm]}{1000 \times SkinDepth[m]}$'"</t>
+  </si>
+  <si>
+    <t>8.69 * P[3] / (1000*sympy.Pow((2)/(2*sympy.pi*P[0]*P[1]*P[2]),0.5))</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Cu Conductivity:Cu Thickness[mm]</t>
+  </si>
+  <si>
+    <t>Abosrption Loss (Al) [dB]</t>
+  </si>
+  <si>
+    <t>Abosrption Loss (Fe) [dB]</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Fe Conductivity:Fe Thickness[mm]</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Al Conductivity:Al Thickness[mm]</t>
+  </si>
+  <si>
+    <t>"r'$Absorption Loss (Al) [dB] = 8.69 \times \frac{Sheild Thickness [mm]}{1000 \times SkinDepth[m]}$'"</t>
+  </si>
+  <si>
+    <t>"r'$Absorption Loss (Fe) [dB] = 8.69 \times \frac{Sheild Thickness [mm]}{1000 \times SkinDepth[m]}$'"</t>
   </si>
 </sst>
 </file>
@@ -1357,7 +1423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1376,6 +1442,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1695,11 +1767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q130"/>
+  <dimension ref="A1:Q136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I136" sqref="I136"/>
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J140" sqref="J140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1708,12 +1780,12 @@
     <col min="2" max="2" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.46484375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14" style="1" customWidth="1"/>
     <col min="9" max="9" width="89.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="102.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="132.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.265625" style="1" bestFit="1" customWidth="1"/>
@@ -6493,7 +6565,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>10</v>
@@ -6528,7 +6600,7 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>10</v>
@@ -6561,9 +6633,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>10</v>
@@ -6596,9 +6668,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>10</v>
@@ -6629,6 +6701,297 @@
       </c>
       <c r="M130" s="1">
         <v>340</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="L131" s="1">
+        <v>1</v>
+      </c>
+      <c r="M131" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="N131" s="8">
+        <v>1.25664E-6</v>
+      </c>
+      <c r="O131" s="7">
+        <v>58000000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="1">
+        <v>131</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="K132" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="L132" s="1">
+        <v>1</v>
+      </c>
+      <c r="M132" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="N132" s="8">
+        <v>1.2566650000000001E-6</v>
+      </c>
+      <c r="O132" s="7">
+        <v>64100000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="1">
+        <v>132</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="K133" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="L133" s="1">
+        <v>1</v>
+      </c>
+      <c r="M133" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="N133" s="8">
+        <v>6.3E-3</v>
+      </c>
+      <c r="O133" s="7">
+        <v>11200000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="1">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="K134" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="L134" s="1">
+        <v>1</v>
+      </c>
+      <c r="M134" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="N134" s="8">
+        <v>1.25664E-6</v>
+      </c>
+      <c r="O134" s="7">
+        <v>58000000</v>
+      </c>
+      <c r="P134" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="J135" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="L135" s="1">
+        <v>1</v>
+      </c>
+      <c r="M135" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="N135" s="8">
+        <v>1.2566650000000001E-6</v>
+      </c>
+      <c r="O135" s="7">
+        <v>64100000</v>
+      </c>
+      <c r="P135" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="1">
+        <v>133</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="J136" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="L136" s="1">
+        <v>1</v>
+      </c>
+      <c r="M136" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="N136" s="8">
+        <v>6.3E-3</v>
+      </c>
+      <c r="O136" s="7">
+        <v>11200000</v>
+      </c>
+      <c r="P136" s="6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Supporting up to 8 parameters
</commit_message>
<xml_diff>
--- a/Converter/assets/UnitConversion.xlsx
+++ b/Converter/assets/UnitConversion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d78e2062db64e14/Project/Python/AnalysisTool/Converter/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://photonicinc-my.sharepoint.com/personal/iyoneda_photonic_com/Documents/Python/AnalysisTool/Converter/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{28AA09F0-1BFD-4629-8D14-FBC6BDF866C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{035093EF-A928-4F0C-9420-79F400ECAB0C}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="13_ncr:1_{28AA09F0-1BFD-4629-8D14-FBC6BDF866C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DD25DB5-AE1F-4CE7-99D1-758051BC4E8E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="14550" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elec" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="464">
   <si>
     <t>No</t>
   </si>
@@ -1303,15 +1303,6 @@
     <t>"r'$SkinDepth (Al)[m] = \sqrt{\frac{2}{2\pi Frequency[Hz] \times Permetivity {\mu} [H/m] \times Conductibity \sigma[S/m]}}$'"</t>
   </si>
   <si>
-    <t>Freq Permeability:Cu Conductivity:Cu</t>
-  </si>
-  <si>
-    <t>Freq Permeability:Al Conductivity:Al</t>
-  </si>
-  <si>
-    <t>Freq Permeability:Fe Conductivity:Fe</t>
-  </si>
-  <si>
     <t>"r'$SkinDepth (Fe)[m] = \sqrt{\frac{2}{2\pi Frequency[Hz] \times Permetivity {\mu} [H/m] \times Conductibity \sigma[S/m]}}$'"</t>
   </si>
   <si>
@@ -1327,25 +1318,125 @@
     <t>8.69 * P[3] / (1000*sympy.Pow((2)/(2*sympy.pi*P[0]*P[1]*P[2]),0.5))</t>
   </si>
   <si>
-    <t>Freq Permeability:Cu Conductivity:Cu Thickness[mm]</t>
-  </si>
-  <si>
     <t>Abosrption Loss (Al) [dB]</t>
   </si>
   <si>
     <t>Abosrption Loss (Fe) [dB]</t>
   </si>
   <si>
-    <t>Freq Permeability:Fe Conductivity:Fe Thickness[mm]</t>
-  </si>
-  <si>
-    <t>Freq Permeability:Al Conductivity:Al Thickness[mm]</t>
-  </si>
-  <si>
     <t>"r'$Absorption Loss (Al) [dB] = 8.69 \times \frac{Sheild Thickness [mm]}{1000 \times SkinDepth[m]}$'"</t>
   </si>
   <si>
     <t>"r'$Absorption Loss (Fe) [dB] = 8.69 \times \frac{Sheild Thickness [mm]}{1000 \times SkinDepth[m]}$'"</t>
+  </si>
+  <si>
+    <t>Freq r:Distance[mm] Relative_Conductivity:sigma Relative_permeability:mu</t>
+  </si>
+  <si>
+    <t>Reflection Loss- Electric Field (Cu) [dB]</t>
+  </si>
+  <si>
+    <t>sympy.Piecewise(
+(14.6 +  10* sympy.log((P[0]*sympy.Pow((P[1]/1000),2)*P[2]/P[3]),10)
+,P[1]&lt;(299792458*1000/(P[0]*2*sympy.pi)))
+,
+(168 + 10 *sympy.log(P[2]/(P[3]*P[0]),10)
+, P[1]&gt;=(299792458*1000/(P[0]*2*sympy.pi)))
+)</t>
+  </si>
+  <si>
+    <t>"r'$Reflection Loss[dB] = \left\{
+\begin{array}{ll}
+14.6 + 10 \log_{10}{\frac{Freq[Hz] \times (Distance(r)[m])^2 \times \sigma_{r}}{\mu_{r}}} &amp; (r \lt \frac{\lambda}{2\pi})\\
+ 168 + 10 \log _{10}(\frac{\sigma_{r}}{\mu_{r} \times Freq[Hz]}) &amp; (r \geq \frac{\lambda}{2\pi})
+\end{array}
+\right.$'"</t>
+  </si>
+  <si>
+    <t>Reflection Loss- Magnetic Field (Cu) [dB]</t>
+  </si>
+  <si>
+    <t>Reflection Loss- Magnetic Field (Fe) [dB]</t>
+  </si>
+  <si>
+    <t>Reflection Loss- Magnetic Field (Al) [dB]</t>
+  </si>
+  <si>
+    <t>sympy.Piecewise(
+(322 +  10* sympy.log((P[2]/(P[3]*sympy.Pow(P[0],3)*sympy.Pow((P[1]/1000),2))),10)
+,P[1]&lt;(299792458*1000/(P[0]*2*sympy.pi)))
+,
+(168 + 10 *sympy.log(P[2]/(P[3]*P[0]),10)
+, P[1]&gt;=(299792458*1000/(P[0]*2*sympy.pi)))
+)</t>
+  </si>
+  <si>
+    <t>"r'$Reflection Loss[dB] = \left\{
+\begin{array}{ll}
+322 + 10 \log_{10}{\frac{\sigma_{r}}{\mu_{r} \times (Freq[Hz])^3 \times (Distance (r)[m])^2}} &amp; (r \lt \frac{\lambda}{2\pi})\\
+ 168 + 10 \log _{10}(\frac{\sigma_{r}}{\mu_{r} \times Freq[Hz]}) &amp; (r \geq \frac{\lambda}{2\pi})
+\end{array}
+\right.$'"</t>
+  </si>
+  <si>
+    <t>Reflection Loss- Electric Field (Al) [dB]</t>
+  </si>
+  <si>
+    <t>Reflection Loss- Electric Field (Fe) [dB]</t>
+  </si>
+  <si>
+    <t>Multiple Reflection Loss- (Cu) [dB]</t>
+  </si>
+  <si>
+    <t>"r'$Multiple Reflection Loss [dB] = 20 \times \log _{10}(1- e^{\frac{-2 Thickness[m]}{Skin Depth[m]}}) $'"</t>
+  </si>
+  <si>
+    <t>20*sympy.log((1-sympy.Pow(sympy.E, (-2*(P[3]/1000)/(sympy.Pow((2)/(2*sympy.pi*P[0]*P[1]*P[2]),0.5))))),10)</t>
+  </si>
+  <si>
+    <t>Multiple Reflection Loss- (Al) [dB]</t>
+  </si>
+  <si>
+    <t>Multiple Reflection Loss- (Fe) [dB]</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Cu[H/m] Conductivity:Cu[S/m]</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Al[H/m] Conductivity:Al[S/m]</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Fe[H/m] Conductivity:Fe[S/m]</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Cu[H/m] Conductivity:Cu[S/m] Thickness[mm]</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Al[H/m] Conductivity:Al[S/m] Thickness[mm]</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Fe[H/m] Conductivity:Fe[S/m] Thickness[mm]</t>
+  </si>
+  <si>
+    <t>Default Param6</t>
+  </si>
+  <si>
+    <t>Default Param7</t>
+  </si>
+  <si>
+    <t>Default Param8</t>
+  </si>
+  <si>
+    <t>Shield Effectiveness-Electric Field (Fe) [dB]</t>
+  </si>
+  <si>
+    <t>"r'$Sheild Effectiveness[dB] = Absorption Loss[dB] + Reflection Loss[dB] + Mulple Reflection Loss [dB] $'"</t>
+  </si>
+  <si>
+    <t>Freq Permeability:Fe[H/m] Conductivity:Fe[S/m] Relative_Conductivity:sigma Relative_permeability:mu ShieldThickness[mm] r:Distance[mm]</t>
+  </si>
+  <si>
+    <t>sympy.log(sympy.Pow(10,(8.69 * P[5] / (1000*sympy.Pow((2)/(2*sympy.pi*P[0]*P[1]*P[2]),0.5)))),10)</t>
   </si>
 </sst>
 </file>
@@ -1423,7 +1514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1448,6 +1539,15 @@
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1767,33 +1867,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q136"/>
+  <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J140" sqref="J140"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I147" sqref="I147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14" style="1" customWidth="1"/>
-    <col min="9" max="9" width="89.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="132.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="14.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.06640625" style="5"/>
+    <col min="9" max="9" width="121" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="132.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="14.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.08984375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="37" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1818,7 +1918,7 @@
       <c r="H1" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1845,8 +1945,17 @@
       <c r="Q1" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R1" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1888,8 +1997,11 @@
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1929,8 +2041,11 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1967,8 +2082,11 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2006,7 +2124,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2044,7 +2162,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2082,7 +2200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2120,7 +2238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2158,7 +2276,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2196,7 +2314,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2234,7 +2352,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2274,8 +2392,11 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2315,8 +2436,11 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2361,8 +2485,11 @@
       </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2399,8 +2526,11 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2440,8 +2570,11 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2478,8 +2611,11 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2516,8 +2652,11 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2554,8 +2693,11 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2592,8 +2734,11 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2630,8 +2775,11 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2666,7 +2814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2701,7 +2849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2738,8 +2886,11 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2776,8 +2927,11 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2812,7 +2966,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2853,7 +3007,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2891,7 +3045,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2929,7 +3083,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2967,7 +3121,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3005,7 +3159,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3043,7 +3197,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3078,7 +3232,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3116,7 +3270,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3157,7 +3311,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3195,7 +3349,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3236,7 +3390,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3277,7 +3431,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3318,7 +3472,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3356,7 +3510,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3394,7 +3548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3435,7 +3589,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3473,7 +3627,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3508,7 +3662,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3543,7 +3697,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3581,7 +3735,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3619,7 +3773,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3657,7 +3811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3695,7 +3849,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3733,7 +3887,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3771,7 +3925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3809,7 +3963,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3847,7 +4001,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3888,7 +4042,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3929,7 +4083,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3970,7 +4124,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4011,7 +4165,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4052,7 +4206,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4093,7 +4247,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4131,7 +4285,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4171,8 +4325,11 @@
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4215,8 +4372,11 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4256,8 +4416,11 @@
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4295,7 +4458,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4335,8 +4498,11 @@
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4376,8 +4542,11 @@
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4420,8 +4589,11 @@
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4456,7 +4628,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4494,7 +4666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4532,7 +4704,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4570,7 +4742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4608,7 +4780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4646,7 +4818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4684,7 +4856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4719,7 +4891,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4760,7 +4932,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -4801,7 +4973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -4842,7 +5014,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -4880,7 +5052,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -4915,7 +5087,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4958,8 +5130,11 @@
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -4996,8 +5171,11 @@
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -5039,8 +5217,11 @@
       </c>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -5078,7 +5259,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -5116,7 +5297,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5151,7 +5332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5186,7 +5367,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5221,7 +5402,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5256,7 +5437,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5291,7 +5472,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5326,7 +5507,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5361,7 +5542,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5396,7 +5577,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5431,7 +5612,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5466,7 +5647,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5501,7 +5682,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -5536,7 +5717,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -5571,7 +5752,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -5606,7 +5787,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -5641,7 +5822,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -5676,7 +5857,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -5711,7 +5892,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -5746,7 +5927,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -5781,7 +5962,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -5816,7 +5997,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -5851,7 +6032,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -5886,7 +6067,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -5921,7 +6102,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -5956,7 +6137,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -5991,7 +6172,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -6026,7 +6207,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -6061,7 +6242,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -6096,7 +6277,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -6131,7 +6312,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -6166,7 +6347,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -6201,7 +6382,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -6236,7 +6417,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -6271,7 +6452,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -6306,7 +6487,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -6344,7 +6525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -6382,7 +6563,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -6417,7 +6598,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -6452,7 +6633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -6493,7 +6674,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -6528,7 +6709,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -6563,7 +6744,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -6598,7 +6779,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -6633,7 +6814,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -6668,7 +6849,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -6703,7 +6884,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -6735,13 +6916,13 @@
         <v>424</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>426</v>
+        <v>451</v>
       </c>
       <c r="L131" s="1">
         <v>1</v>
       </c>
       <c r="M131" s="1">
-        <v>1000000000</v>
+        <v>20000000000</v>
       </c>
       <c r="N131" s="8">
         <v>1.25664E-6</v>
@@ -6750,7 +6931,7 @@
         <v>58000000</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -6782,13 +6963,13 @@
         <v>425</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>427</v>
+        <v>452</v>
       </c>
       <c r="L132" s="1">
         <v>1</v>
       </c>
       <c r="M132" s="1">
-        <v>1000000000</v>
+        <v>20000000000</v>
       </c>
       <c r="N132" s="8">
         <v>1.2566650000000001E-6</v>
@@ -6797,7 +6978,7 @@
         <v>64100000</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -6811,7 +6992,7 @@
         <v>420</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>307</v>
@@ -6826,16 +7007,16 @@
         <v>422</v>
       </c>
       <c r="J133" s="2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>428</v>
+        <v>453</v>
       </c>
       <c r="L133" s="1">
         <v>1</v>
       </c>
       <c r="M133" s="1">
-        <v>1000000000</v>
+        <v>20000000000</v>
       </c>
       <c r="N133" s="8">
         <v>6.3E-3</v>
@@ -6844,7 +7025,7 @@
         <v>11200000</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -6858,7 +7039,7 @@
         <v>420</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>88</v>
@@ -6870,19 +7051,19 @@
         <v>192</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>434</v>
+        <v>454</v>
       </c>
       <c r="L134" s="1">
         <v>1</v>
       </c>
       <c r="M134" s="1">
-        <v>1000000000</v>
+        <v>20000000000</v>
       </c>
       <c r="N134" s="8">
         <v>1.25664E-6</v>
@@ -6891,12 +7072,12 @@
         <v>58000000</v>
       </c>
       <c r="P134" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A135" s="1">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>102</v>
@@ -6908,7 +7089,7 @@
         <v>420</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>88</v>
@@ -6920,19 +7101,19 @@
         <v>192</v>
       </c>
       <c r="I135" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="J135" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="J135" s="2" t="s">
-        <v>439</v>
-      </c>
       <c r="K135" s="1" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
       <c r="L135" s="1">
         <v>1</v>
       </c>
       <c r="M135" s="1">
-        <v>1000000000</v>
+        <v>20000000000</v>
       </c>
       <c r="N135" s="8">
         <v>1.2566650000000001E-6</v>
@@ -6941,12 +7122,12 @@
         <v>64100000</v>
       </c>
       <c r="P135" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A136" s="1">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>102</v>
@@ -6958,7 +7139,7 @@
         <v>420</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>88</v>
@@ -6970,19 +7151,19 @@
         <v>192</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J136" s="2" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>437</v>
+        <v>456</v>
       </c>
       <c r="L136" s="1">
         <v>1</v>
       </c>
       <c r="M136" s="1">
-        <v>1000000000</v>
+        <v>20000000000</v>
       </c>
       <c r="N136" s="8">
         <v>6.3E-3</v>
@@ -6991,8 +7172,488 @@
         <v>11200000</v>
       </c>
       <c r="P136" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" ht="129.5" x14ac:dyDescent="0.45">
+      <c r="A137" s="1">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I137" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="J137" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="L137" s="1">
         <v>1</v>
       </c>
+      <c r="M137" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N137" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="O137" s="1">
+        <v>1</v>
+      </c>
+      <c r="P137" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" ht="129.5" x14ac:dyDescent="0.45">
+      <c r="A138" s="1">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I138" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="J138" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="L138" s="1">
+        <v>1</v>
+      </c>
+      <c r="M138" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N138" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="O138" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="P138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" ht="129.5" x14ac:dyDescent="0.45">
+      <c r="A139" s="1">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I139" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="J139" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="L139" s="1">
+        <v>1</v>
+      </c>
+      <c r="M139" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N139" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="O139" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P139" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" ht="129.5" x14ac:dyDescent="0.45">
+      <c r="A140" s="1">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I140" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="J140" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="L140" s="1">
+        <v>1</v>
+      </c>
+      <c r="M140" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N140" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="O140" s="1">
+        <v>1</v>
+      </c>
+      <c r="P140" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" ht="129.5" x14ac:dyDescent="0.45">
+      <c r="A141" s="1">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I141" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="J141" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="L141" s="1">
+        <v>1</v>
+      </c>
+      <c r="M141" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N141" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="O141" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="P141" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" ht="129.5" x14ac:dyDescent="0.45">
+      <c r="A142" s="1">
+        <v>141</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I142" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="J142" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="L142" s="1">
+        <v>1</v>
+      </c>
+      <c r="M142" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N142" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="O142" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P142" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A143" s="1">
+        <v>142</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="J143" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="L143" s="1">
+        <v>1</v>
+      </c>
+      <c r="M143" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N143" s="8">
+        <v>1.25664E-6</v>
+      </c>
+      <c r="O143" s="7">
+        <v>58000000</v>
+      </c>
+      <c r="P143" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A144" s="1">
+        <v>143</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="J144" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="L144" s="1">
+        <v>1</v>
+      </c>
+      <c r="M144" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N144" s="8">
+        <v>1.2566650000000001E-6</v>
+      </c>
+      <c r="O144" s="7">
+        <v>64100000</v>
+      </c>
+      <c r="P144" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A145" s="1">
+        <v>144</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="J145" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="L145" s="1">
+        <v>1</v>
+      </c>
+      <c r="M145" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N145" s="8">
+        <v>6.3E-3</v>
+      </c>
+      <c r="O145" s="7">
+        <v>11200000</v>
+      </c>
+      <c r="P145" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" ht="55.5" x14ac:dyDescent="0.45">
+      <c r="A146" s="1">
+        <v>145</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="J146" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="K146" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="L146" s="1">
+        <v>1</v>
+      </c>
+      <c r="M146" s="1">
+        <v>20000000000</v>
+      </c>
+      <c r="N146" s="8">
+        <v>6.3E-3</v>
+      </c>
+      <c r="O146" s="8">
+        <v>11200000</v>
+      </c>
+      <c r="P146" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="Q146" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R146" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="S146" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="T146" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q123" xr:uid="{00000000-0001-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Added Vp to dBm
</commit_message>
<xml_diff>
--- a/Converter/assets/UnitConversion.xlsx
+++ b/Converter/assets/UnitConversion.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d78e2062db64e14/Project/Python/AnalysisTool/Converter/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://photonicinc-my.sharepoint.com/personal/iyoneda_photonic_com/Documents/Python/AnalysisTool/Converter/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{125855ED-4C9C-420F-91B7-F40C5A158F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D404822-27CB-417F-903C-E4236564FF84}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{125855ED-4C9C-420F-91B7-F40C5A158F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7904583-99D3-4AC3-B85A-528E6304B311}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26172" yWindow="2220" windowWidth="21324" windowHeight="12768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elec" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elec!$A$1:$Q$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elec!$A$1:$Q$157</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="502">
   <si>
     <t>No</t>
   </si>
@@ -1654,6 +1654,21 @@
 43.5 dB{\mu}V/m &amp; (\geq 1000[ MHz] ) \\
 \end{array}
 \right.$'"</t>
+  </si>
+  <si>
+    <t>"r$Watt[dBm] = 10 \times \log _{10}(\frac{Voltage[Vp]^2 \times 1000}{2 \times Z})$"</t>
+  </si>
+  <si>
+    <t>Vpeak Z</t>
+  </si>
+  <si>
+    <t>10 * sympy.log(((P[0]**2 * 1000) /(2*P[1])), 10)</t>
+  </si>
+  <si>
+    <t>sympy.Pow((2*P[1]/1000),0.5) * sympy.Pow(10, P[0]/20)</t>
+  </si>
+  <si>
+    <t>"r'$Voltage[V] = \sqrt{\frac{2Z}{1000}} \times 10^\frac{Watt[dBm]}{20}$'"</t>
   </si>
 </sst>
 </file>
@@ -2081,36 +2096,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T156"/>
+  <dimension ref="A1:T158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M156" sqref="M156"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K175" sqref="K175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="28.5" x14ac:dyDescent="0.85"/>
+  <sheetFormatPr defaultColWidth="9.05078125" defaultRowHeight="28.2" x14ac:dyDescent="1.05"/>
   <cols>
-    <col min="1" max="1" width="13.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="183.46484375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="207.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="195.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="21.73046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.19921875" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.06640625" style="6"/>
+    <col min="1" max="1" width="13.83984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1015625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.3125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.20703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="183.47265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="207.7890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="195.7890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.26171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.26171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="21.734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.20703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.83984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.05078125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="84.6" x14ac:dyDescent="1.05">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2187,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2222,7 +2237,7 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="3" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2272,7 +2287,7 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="4" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2322,7 +2337,7 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="5" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2363,7 +2378,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="6" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2398,7 +2413,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="171" x14ac:dyDescent="0.85">
+    <row r="7" spans="1:20" ht="169.2" x14ac:dyDescent="1.05">
       <c r="A7" s="4">
         <v>152</v>
       </c>
@@ -2436,7 +2451,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="171" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:20" ht="169.2" x14ac:dyDescent="1.05">
       <c r="A8" s="4">
         <v>153</v>
       </c>
@@ -2474,7 +2489,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="9" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -2512,7 +2527,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="10" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -2550,7 +2565,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="11" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A11" s="4">
         <v>8</v>
       </c>
@@ -2591,7 +2606,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="12" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -2635,7 +2650,7 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="13" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A13" s="4">
         <v>10</v>
       </c>
@@ -2676,7 +2691,7 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="14" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -2717,7 +2732,7 @@
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="15" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A15" s="4">
         <v>12</v>
       </c>
@@ -2758,7 +2773,7 @@
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="16" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -2799,7 +2814,7 @@
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="17" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A17" s="4">
         <v>14</v>
       </c>
@@ -2840,7 +2855,7 @@
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="18" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A18" s="4">
         <v>15</v>
       </c>
@@ -2881,7 +2896,7 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="19" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A19" s="4">
         <v>16</v>
       </c>
@@ -2922,7 +2937,7 @@
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="20" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -2963,7 +2978,7 @@
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="21" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A21" s="4">
         <v>18</v>
       </c>
@@ -3004,7 +3019,7 @@
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="22" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -3042,7 +3057,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="23" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A23" s="4">
         <v>20</v>
       </c>
@@ -3080,7 +3095,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="24" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A24" s="4">
         <v>21</v>
       </c>
@@ -3121,7 +3136,7 @@
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="25" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A25" s="4">
         <v>22</v>
       </c>
@@ -3165,7 +3180,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="26" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A26" s="4">
         <v>23</v>
       </c>
@@ -3206,7 +3221,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="27" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A27" s="4">
         <v>24</v>
       </c>
@@ -3244,7 +3259,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="28" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -3285,7 +3300,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="29" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A29" s="4">
         <v>26</v>
       </c>
@@ -3326,7 +3341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="30" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A30" s="4">
         <v>27</v>
       </c>
@@ -3367,7 +3382,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="31" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A31" s="4">
         <v>28</v>
       </c>
@@ -3408,7 +3423,7 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="32" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A32" s="4">
         <v>29</v>
       </c>
@@ -3449,7 +3464,7 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="33" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A33" s="4">
         <v>30</v>
       </c>
@@ -3495,7 +3510,7 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="34" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A34" s="4">
         <v>31</v>
       </c>
@@ -3533,7 +3548,7 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="35" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A35" s="4">
         <v>32</v>
       </c>
@@ -3576,7 +3591,7 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="36" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A36" s="4">
         <v>33</v>
       </c>
@@ -3611,7 +3626,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="228" x14ac:dyDescent="0.85">
+    <row r="37" spans="1:17" ht="225.6" x14ac:dyDescent="1.05">
       <c r="A37" s="4">
         <v>34</v>
       </c>
@@ -3649,7 +3664,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="228" x14ac:dyDescent="0.85">
+    <row r="38" spans="1:17" ht="225.6" x14ac:dyDescent="1.05">
       <c r="A38" s="4">
         <v>35</v>
       </c>
@@ -3687,7 +3702,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="171" x14ac:dyDescent="0.85">
+    <row r="39" spans="1:17" ht="169.2" x14ac:dyDescent="1.05">
       <c r="A39" s="4">
         <v>36</v>
       </c>
@@ -3725,7 +3740,7 @@
         <v>50000000</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="171" x14ac:dyDescent="0.85">
+    <row r="40" spans="1:17" ht="169.2" x14ac:dyDescent="1.05">
       <c r="A40" s="4">
         <v>37</v>
       </c>
@@ -3763,7 +3778,7 @@
         <v>50000000</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="228" x14ac:dyDescent="0.85">
+    <row r="41" spans="1:17" ht="225.6" x14ac:dyDescent="1.05">
       <c r="A41" s="4">
         <v>151</v>
       </c>
@@ -3801,7 +3816,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="228" x14ac:dyDescent="0.85">
+    <row r="42" spans="1:17" ht="225.6" x14ac:dyDescent="1.05">
       <c r="A42" s="4">
         <v>150</v>
       </c>
@@ -3839,7 +3854,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="43" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A43" s="4">
         <v>38</v>
       </c>
@@ -3880,7 +3895,7 @@
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="44" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A44" s="4">
         <v>39</v>
       </c>
@@ -3915,7 +3930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="45" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A45" s="4">
         <v>40</v>
       </c>
@@ -3953,7 +3968,7 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="46" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A46" s="4">
         <v>41</v>
       </c>
@@ -3988,7 +4003,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="47" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A47" s="4">
         <v>42</v>
       </c>
@@ -4023,7 +4038,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="48" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A48" s="4">
         <v>43</v>
       </c>
@@ -4058,7 +4073,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="49" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A49" s="4">
         <v>44</v>
       </c>
@@ -4093,7 +4108,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="50" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A50" s="4">
         <v>45</v>
       </c>
@@ -4128,7 +4143,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="51" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A51" s="4">
         <v>46</v>
       </c>
@@ -4163,7 +4178,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="52" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A52" s="4">
         <v>47</v>
       </c>
@@ -4198,7 +4213,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="53" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A53" s="4">
         <v>48</v>
       </c>
@@ -4233,7 +4248,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="54" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A54" s="4">
         <v>49</v>
       </c>
@@ -4268,7 +4283,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="55" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A55" s="4">
         <v>50</v>
       </c>
@@ -4303,7 +4318,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="56" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A56" s="4">
         <v>51</v>
       </c>
@@ -4338,7 +4353,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="57" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A57" s="4">
         <v>52</v>
       </c>
@@ -4373,7 +4388,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="58" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A58" s="4">
         <v>53</v>
       </c>
@@ -4408,7 +4423,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="59" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A59" s="4">
         <v>54</v>
       </c>
@@ -4443,7 +4458,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="60" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A60" s="4">
         <v>55</v>
       </c>
@@ -4478,7 +4493,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="61" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A61" s="4">
         <v>56</v>
       </c>
@@ -4516,7 +4531,7 @@
       <c r="S61" s="4"/>
       <c r="T61" s="4"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="62" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A62" s="4">
         <v>57</v>
       </c>
@@ -4554,7 +4569,7 @@
       <c r="S62" s="4"/>
       <c r="T62" s="4"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="63" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A63" s="4">
         <v>58</v>
       </c>
@@ -4592,7 +4607,7 @@
       <c r="S63" s="4"/>
       <c r="T63" s="4"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="64" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A64" s="4">
         <v>59</v>
       </c>
@@ -4627,7 +4642,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="65" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A65" s="4">
         <v>60</v>
       </c>
@@ -4665,7 +4680,7 @@
       <c r="S65" s="4"/>
       <c r="T65" s="4"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="66" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A66" s="4">
         <v>61</v>
       </c>
@@ -4706,7 +4721,7 @@
       <c r="S66" s="4"/>
       <c r="T66" s="4"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="67" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A67" s="4">
         <v>62</v>
       </c>
@@ -4744,7 +4759,7 @@
       <c r="S67" s="4"/>
       <c r="T67" s="4"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="68" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A68" s="4">
         <v>63</v>
       </c>
@@ -4779,7 +4794,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="69" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A69" s="4">
         <v>64</v>
       </c>
@@ -4814,7 +4829,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="70" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A70" s="4">
         <v>65</v>
       </c>
@@ -4849,7 +4864,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="71" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A71" s="4">
         <v>66</v>
       </c>
@@ -4884,7 +4899,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="72" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A72" s="4">
         <v>67</v>
       </c>
@@ -4919,7 +4934,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="73" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A73" s="4">
         <v>68</v>
       </c>
@@ -4954,7 +4969,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="74" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A74" s="4">
         <v>69</v>
       </c>
@@ -4989,7 +5004,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="75" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A75" s="4">
         <v>70</v>
       </c>
@@ -5024,7 +5039,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="76" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A76" s="4">
         <v>71</v>
       </c>
@@ -5062,7 +5077,7 @@
       <c r="P76" s="4"/>
       <c r="Q76" s="4"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="77" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A77" s="4">
         <v>72</v>
       </c>
@@ -5097,7 +5112,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="78" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A78" s="4">
         <v>73</v>
       </c>
@@ -5132,7 +5147,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="79" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A79" s="4">
         <v>74</v>
       </c>
@@ -5167,7 +5182,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="80" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A80" s="4">
         <v>75</v>
       </c>
@@ -5202,7 +5217,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="81" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A81" s="4">
         <v>76</v>
       </c>
@@ -5240,7 +5255,7 @@
       <c r="S81" s="4"/>
       <c r="T81" s="4"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="82" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A82" s="4">
         <v>77</v>
       </c>
@@ -5281,7 +5296,7 @@
       <c r="S82" s="4"/>
       <c r="T82" s="4"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="83" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A83" s="4">
         <v>78</v>
       </c>
@@ -5319,7 +5334,7 @@
       <c r="P83" s="4"/>
       <c r="Q83" s="4"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="84" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A84" s="4">
         <v>79</v>
       </c>
@@ -5366,7 +5381,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="85" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A85" s="4">
         <v>80</v>
       </c>
@@ -5413,7 +5428,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="86" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A86" s="4">
         <v>81</v>
       </c>
@@ -5460,7 +5475,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="87" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A87" s="4">
         <v>82</v>
       </c>
@@ -5498,7 +5513,7 @@
       <c r="P87" s="4"/>
       <c r="Q87" s="4"/>
     </row>
-    <row r="88" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="88" spans="1:20" ht="197.4" x14ac:dyDescent="1.05">
       <c r="A88" s="4">
         <v>83</v>
       </c>
@@ -5545,7 +5560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="89" spans="1:20" ht="197.4" x14ac:dyDescent="1.05">
       <c r="A89" s="4">
         <v>84</v>
       </c>
@@ -5592,7 +5607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="90" spans="1:20" ht="197.4" x14ac:dyDescent="1.05">
       <c r="A90" s="4">
         <v>85</v>
       </c>
@@ -5639,7 +5654,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="91" spans="1:20" ht="197.4" x14ac:dyDescent="1.05">
       <c r="A91" s="4">
         <v>86</v>
       </c>
@@ -5686,7 +5701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="92" spans="1:20" ht="197.4" x14ac:dyDescent="1.05">
       <c r="A92" s="4">
         <v>87</v>
       </c>
@@ -5733,7 +5748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="93" spans="1:20" ht="197.4" x14ac:dyDescent="1.05">
       <c r="A93" s="4">
         <v>88</v>
       </c>
@@ -5780,7 +5795,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="94" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A94" s="4">
         <v>89</v>
       </c>
@@ -5821,7 +5836,7 @@
       <c r="P94" s="4"/>
       <c r="Q94" s="4"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="95" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A95" s="4">
         <v>90</v>
       </c>
@@ -5862,7 +5877,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="96" spans="1:20" x14ac:dyDescent="1.05">
       <c r="A96" s="4">
         <v>91</v>
       </c>
@@ -5897,7 +5912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="97" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A97" s="4">
         <v>92</v>
       </c>
@@ -5944,7 +5959,7 @@
         <v>64100000</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="98" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A98" s="4">
         <v>93</v>
       </c>
@@ -5991,7 +6006,7 @@
         <v>58000000</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="99" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A99" s="4">
         <v>94</v>
       </c>
@@ -6038,7 +6053,7 @@
         <v>11200000</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="100" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A100" s="4">
         <v>95</v>
       </c>
@@ -6081,7 +6096,7 @@
       <c r="P100" s="4"/>
       <c r="Q100" s="4"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="101" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A101" s="4">
         <v>96</v>
       </c>
@@ -6119,7 +6134,7 @@
       <c r="P101" s="4"/>
       <c r="Q101" s="4"/>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="102" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A102" s="4">
         <v>97</v>
       </c>
@@ -6154,7 +6169,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="103" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A103" s="4">
         <v>98</v>
       </c>
@@ -6192,7 +6207,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="104" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A104" s="4">
         <v>99</v>
       </c>
@@ -6230,7 +6245,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="105" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A105" s="4">
         <v>100</v>
       </c>
@@ -6265,7 +6280,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="106" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A106" s="4">
         <v>101</v>
       </c>
@@ -6300,7 +6315,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="107" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A107" s="4">
         <v>102</v>
       </c>
@@ -6341,7 +6356,7 @@
       <c r="P107" s="4"/>
       <c r="Q107" s="4"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="108" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A108" s="4">
         <v>103</v>
       </c>
@@ -6382,7 +6397,7 @@
       <c r="P108" s="4"/>
       <c r="Q108" s="4"/>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="109" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A109" s="4">
         <v>104</v>
       </c>
@@ -6417,7 +6432,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="110" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A110" s="4">
         <v>105</v>
       </c>
@@ -6455,7 +6470,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="111" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A111" s="4">
         <v>106</v>
       </c>
@@ -6493,7 +6508,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="112" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A112" s="4">
         <v>107</v>
       </c>
@@ -6531,7 +6546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="113" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A113" s="4">
         <v>108</v>
       </c>
@@ -6569,7 +6584,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="114" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A114" s="4">
         <v>109</v>
       </c>
@@ -6610,7 +6625,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="115" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A115" s="4">
         <v>110</v>
       </c>
@@ -6648,7 +6663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="116" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A116" s="4">
         <v>111</v>
       </c>
@@ -6686,7 +6701,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="117" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A117" s="4">
         <v>112</v>
       </c>
@@ -6727,7 +6742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="118" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A118" s="4">
         <v>113</v>
       </c>
@@ -6765,7 +6780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="119" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A119" s="4">
         <v>114</v>
       </c>
@@ -6803,7 +6818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="120" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A120" s="4">
         <v>115</v>
       </c>
@@ -6841,7 +6856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="121" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A121" s="4">
         <v>116</v>
       </c>
@@ -6885,7 +6900,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="122" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A122" s="4">
         <v>117</v>
       </c>
@@ -6920,7 +6935,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="123" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A123" s="4">
         <v>118</v>
       </c>
@@ -6955,7 +6970,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="124" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A124" s="4">
         <v>119</v>
       </c>
@@ -6990,7 +7005,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="125" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A125" s="4">
         <v>120</v>
       </c>
@@ -7034,7 +7049,7 @@
       <c r="P125" s="4"/>
       <c r="Q125" s="4"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="126" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A126" s="4">
         <v>121</v>
       </c>
@@ -7078,7 +7093,7 @@
       <c r="P126" s="4"/>
       <c r="Q126" s="4"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="127" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A127" s="4">
         <v>122</v>
       </c>
@@ -7113,7 +7128,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="128" spans="1:17" x14ac:dyDescent="1.05">
       <c r="A128" s="4">
         <v>123</v>
       </c>
@@ -7148,7 +7163,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="129" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A129" s="4">
         <v>124</v>
       </c>
@@ -7183,7 +7198,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="130" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A130" s="4">
         <v>125</v>
       </c>
@@ -7221,7 +7236,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="131" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A131" s="4">
         <v>126</v>
       </c>
@@ -7259,7 +7274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="132" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A132" s="4">
         <v>127</v>
       </c>
@@ -7297,7 +7312,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="133" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A133" s="4">
         <v>128</v>
       </c>
@@ -7338,7 +7353,7 @@
       <c r="P133" s="4"/>
       <c r="Q133" s="4"/>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="134" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A134" s="4">
         <v>129</v>
       </c>
@@ -7373,7 +7388,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="135" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A135" s="4">
         <v>130</v>
       </c>
@@ -7411,7 +7426,7 @@
       <c r="P135" s="4"/>
       <c r="Q135" s="4"/>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="136" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A136" s="4">
         <v>131</v>
       </c>
@@ -7449,7 +7464,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="137" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A137" s="4">
         <v>132</v>
       </c>
@@ -7487,7 +7502,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="138" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A138" s="4">
         <v>133</v>
       </c>
@@ -7522,7 +7537,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="139" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A139" s="4">
         <v>134</v>
       </c>
@@ -7560,7 +7575,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="140" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A140" s="4">
         <v>135</v>
       </c>
@@ -7598,7 +7613,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="141" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A141" s="4">
         <v>136</v>
       </c>
@@ -7633,7 +7648,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="142" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A142" s="4">
         <v>137</v>
       </c>
@@ -7671,7 +7686,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="143" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A143" s="4">
         <v>138</v>
       </c>
@@ -7712,7 +7727,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="144" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A144" s="4">
         <v>139</v>
       </c>
@@ -7756,7 +7771,7 @@
         <v>11200000</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="145" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A145" s="4">
         <v>140</v>
       </c>
@@ -7800,7 +7815,7 @@
         <v>11200000</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="146" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A146" s="4">
         <v>141</v>
       </c>
@@ -7841,7 +7856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="147" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A147" s="4">
         <v>142</v>
       </c>
@@ -7879,7 +7894,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="148" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A148" s="4">
         <v>143</v>
       </c>
@@ -7920,7 +7935,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="149" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A149" s="4">
         <v>144</v>
       </c>
@@ -7961,7 +7976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="150" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A150" s="4">
         <v>145</v>
       </c>
@@ -8005,7 +8020,7 @@
       <c r="P150" s="4"/>
       <c r="Q150" s="4"/>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="151" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A151" s="4">
         <v>146</v>
       </c>
@@ -8043,7 +8058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="152" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A152" s="4">
         <v>147</v>
       </c>
@@ -8081,7 +8096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="153" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A153" s="4">
         <v>148</v>
       </c>
@@ -8119,7 +8134,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.85">
+    <row r="154" spans="1:18" x14ac:dyDescent="1.05">
       <c r="A154" s="4">
         <v>149</v>
       </c>
@@ -8157,7 +8172,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="155" spans="1:18" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="155" spans="1:18" ht="197.4" x14ac:dyDescent="1.05">
+      <c r="A155" s="4">
+        <v>150</v>
+      </c>
       <c r="B155" s="4" t="s">
         <v>126</v>
       </c>
@@ -8192,7 +8210,10 @@
         <v>10000000000</v>
       </c>
     </row>
-    <row r="156" spans="1:18" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="156" spans="1:18" ht="197.4" x14ac:dyDescent="1.05">
+      <c r="A156" s="4">
+        <v>151</v>
+      </c>
       <c r="B156" s="4" t="s">
         <v>126</v>
       </c>
@@ -8227,8 +8248,93 @@
         <v>10000000000</v>
       </c>
     </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="1.05">
+      <c r="A157" s="4">
+        <v>152</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F157" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I157" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="J157" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="K157" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="L157" s="4">
+        <v>0</v>
+      </c>
+      <c r="M157" s="4">
+        <v>100</v>
+      </c>
+      <c r="N157" s="4">
+        <v>50</v>
+      </c>
+      <c r="O157" s="4"/>
+      <c r="P157" s="4"/>
+      <c r="Q157" s="4"/>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="1.05">
+      <c r="A158" s="4">
+        <v>153</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="F158" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="H158" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I158" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="J158" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="K158" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L158" s="4">
+        <v>-120</v>
+      </c>
+      <c r="M158" s="4">
+        <v>50</v>
+      </c>
+      <c r="N158" s="4">
+        <v>50</v>
+      </c>
+      <c r="O158" s="4"/>
+      <c r="P158" s="4"/>
+      <c r="Q158" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q156" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:Q157" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q154">
       <sortCondition ref="E1:E154"/>
     </sortState>

</xml_diff>

<commit_message>
Unit Conversion Sheet Update
</commit_message>
<xml_diff>
--- a/Converter/assets/UnitConversion.xlsx
+++ b/Converter/assets/UnitConversion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d78e2062db64e14/Project/Python/AnalysisTool/Converter/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{125855ED-4C9C-420F-91B7-F40C5A158F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D404822-27CB-417F-903C-E4236564FF84}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{4B2675F5-5A15-4F18-A563-C3F38DCA542D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AAEDA61-E197-474E-ADE2-0607CD0AE363}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Elec" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elec!$A$1:$Q$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elec!$A$1:$Q$157</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="546">
   <si>
     <t>No</t>
   </si>
@@ -1654,6 +1654,160 @@
 43.5 dB{\mu}V/m &amp; (\geq 1000[ MHz] ) \\
 \end{array}
 \right.$'"</t>
+  </si>
+  <si>
+    <t>"r$Watt[dBm] = 10 \times \log _{10}(\frac{Voltage[Vp]^2 \times 1000}{2 \times Z})$"</t>
+  </si>
+  <si>
+    <t>Vpeak Z</t>
+  </si>
+  <si>
+    <t>10 * sympy.log(((P[0]**2 * 1000) /(2*P[1])), 10)</t>
+  </si>
+  <si>
+    <t>sympy.Pow((2*P[1]/1000),0.5) * sympy.Pow(10, P[0]/20)</t>
+  </si>
+  <si>
+    <t>"r'$Voltage[V] = \sqrt{\frac{2Z}{1000}} \times 10^\frac{Watt[dBm]}{20}$'"</t>
+  </si>
+  <si>
+    <t>[F/m]</t>
+  </si>
+  <si>
+    <t>Effective Relative Permittivity [F/m]</t>
+  </si>
+  <si>
+    <t>[F/m] Width[mm] Height[mm]</t>
+  </si>
+  <si>
+    <t>(P[0]+1)/2 + ((P[0]-1)/2)*sympy.Pow(1+10*(P[2]/1e3)/(P[1]/1e3),-1*(1+1/49*sympy.log((sympy.Pow(((P[1]/1e3)/(P[2]/1e3)),4) + sympy.Pow(((P[1]/1e3)/(52*(P[2]/1e3))),2))/(sympy.Pow(((P[1]/1e3)/(P[2]/1e3)),4) + 0.432))) + 1/18.7 * sympy.log(1+sympy.Pow((P[1]/1e3)/(18.1*(P[2]/1e3)),3)) * 0.564*sympy.Pow((P[0]-0.9)/(P[0]+3),0.053))</t>
+  </si>
+  <si>
+    <t>"r'$\begin{array}{ll}
+Effective Permittivity:\varepsilon_\mathrm{e}[F/m] = \frac{\varepsilon_\mathrm{r}+1}{2} + \frac{\varepsilon_\mathrm{r}-1}{2} \times\lbrack1+\frac{10\times Height[mm]}{Width[mm]}\rbrack^{-ab} \\
+a=1+\frac{1}{49}ln\lbrack\frac{\frac{Width}{Height}^{4} + \frac{Width}{52\times Height}^2}{\frac{Width}{Height}^{4} + 0.432}\rbrack  + \frac{1}{18.7}ln\lbrack 1+(\frac{Width}{18.1 \times Height})^3 \rbrack\\
+b=0.564\lbrack\frac{\varepsilon_\mathrm{r}-0.9}{\varepsilon_\mathrm{r}+3}\rbrack^{0.053} \\
+\end{array}$'"</t>
+  </si>
+  <si>
+    <t>Width [mm]</t>
+  </si>
+  <si>
+    <t>Width[mm] Effective-Permittivity[F/m] Height[mm]</t>
+  </si>
+  <si>
+    <t>Height [mm]</t>
+  </si>
+  <si>
+    <t>Height[mm] Effective-Permittivity[F/m] Width[mm]</t>
+  </si>
+  <si>
+    <t>(P[1]+1)/2 + ((P[1]-1)/2)*sympy.Pow(1+10*(P[0]/1e3)/(P[2]/1e3),-1*(1+1/49*sympy.log((sympy.Pow(((P[2]/1e3)/(P[0]/1e3)),4) + sympy.Pow(((P[2]/1e3)/(52*(P[0]/1e3))),2))/(sympy.Pow(((P[2]/1e3)/(P[0]/1e3)),4) + 0.432))) + 1/18.7 * sympy.log(1+sympy.Pow((P[2]/1e3)/(18.1*(P[0]/1e3)),3)) * 0.564*sympy.Pow((P[1]-0.9)/(P[1]+3),0.053))</t>
+  </si>
+  <si>
+    <t>(P[1]+1)/2 + ((P[1]-1)/2)*sympy.Pow(1+10*(P[2]/1e3)/(P[0]/1e3),-1*(1+1/49*sympy.log((sympy.Pow(((P[0]/1e3)/(P[2]/1e3)),4) + sympy.Pow(((P[0]/1e3)/(52*(P[2]/1e3))),2))/(sympy.Pow(((P[0]/1e3)/(P[2]/1e3)),4) + 0.432))) + 1/18.7 * sympy.log(1+sympy.Pow((P[0]/1e3)/(18.1*(P[2]/1e3)),3)) * 0.564*sympy.Pow((P[1]-0.9)/(P[1]+3),0.053))</t>
+  </si>
+  <si>
+    <t>Air Impedance [ohm]</t>
+  </si>
+  <si>
+    <t>Relative Permittivity [F/m]</t>
+  </si>
+  <si>
+    <t>[ohm]</t>
+  </si>
+  <si>
+    <t>Width[mm] Height[mm]</t>
+  </si>
+  <si>
+    <t>60 * sympy.ln(6+(2*sympy.pi-6)*sympy.exp(-1*sympy.Pow(30.666*(P[1]/1e3)/(P[0]/1e3),0.7528)) + sympy.Pow(1+sympy.Pow(2*(P[1]/1e3)/(P[0]/1e3),2),0.5))*(P[1]/1e3)/(P[0]/1e3)</t>
+  </si>
+  <si>
+    <t>"r'$\begin{array}{ll}
+Z_0|_{air} = 60ln\left[ \frac{F_1 \times Height[mm]}{Width[mm} \sqrt{1 + (\frac{2* Height[mm]}{Width[mm})^2} \right] \\
+F_1 = 6 + (2\pi-6)exp\left[ -(\frac{30.666 Height[mm]}{Width[mm]})^{0.7528} \right] \\
+\end{array}$'"</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>[g]</t>
+  </si>
+  <si>
+    <t>Once [oz]</t>
+  </si>
+  <si>
+    <t>Gram [g]</t>
+  </si>
+  <si>
+    <t>P[0] / 28.3495</t>
+  </si>
+  <si>
+    <t>Gram[g]</t>
+  </si>
+  <si>
+    <t>"r'$Once[oz] = \frac{Grams[g]}{28.3495}$'"</t>
+  </si>
+  <si>
+    <t>P[0] * 28.3495</t>
+  </si>
+  <si>
+    <t>"r'$Gram[g] = 28.3495 \times Grams[g]$'"</t>
+  </si>
+  <si>
+    <t>Once[oz]</t>
+  </si>
+  <si>
+    <t>Once per square foot</t>
+  </si>
+  <si>
+    <t>[oz/ft^2]</t>
+  </si>
+  <si>
+    <t>Copper Thickness [um]</t>
+  </si>
+  <si>
+    <t>[um]</t>
+  </si>
+  <si>
+    <t>P[0] * 34.79</t>
+  </si>
+  <si>
+    <t>"r'$Copper Thickness[{\mu}m] = 34.79 \times Once per square foot[oz/ft^2]$'"</t>
+  </si>
+  <si>
+    <t>Once-per-square-foot[oz/ft^2]</t>
+  </si>
+  <si>
+    <t>P[0] / 34.79</t>
+  </si>
+  <si>
+    <t>"r'$Copper Thickness[{\mu}m] = \frac{Once per square foot[oz/ft^2]}{34.79}$'"</t>
+  </si>
+  <si>
+    <t>Copper-Thickness[um]</t>
+  </si>
+  <si>
+    <t>Pound [lb]</t>
+  </si>
+  <si>
+    <t>[lb]</t>
+  </si>
+  <si>
+    <t>P[0] / 453.592</t>
+  </si>
+  <si>
+    <t>"r'$Pound[lb] = \frac{Grams[g]}{453.592}$'"</t>
+  </si>
+  <si>
+    <t>P[0] * 453.593</t>
+  </si>
+  <si>
+    <t>"r'$Gram[g] = 453.592 \times Pound[lb]$'"</t>
+  </si>
+  <si>
+    <t>Pound[lb]</t>
   </si>
 </sst>
 </file>
@@ -1731,7 +1885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1751,16 +1905,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2081,21 +2232,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T156"/>
+  <dimension ref="A1:T168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M156" sqref="M156"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="51" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M169" sqref="M169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="28.5" x14ac:dyDescent="0.85"/>
   <cols>
-    <col min="1" max="1" width="13.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.06640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="74.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.06640625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.19921875" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="183.46484375" style="4" bestFit="1" customWidth="1"/>
@@ -2103,10 +2254,9 @@
     <col min="11" max="11" width="195.796875" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.265625" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="21.73046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.19921875" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="21.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.796875" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
@@ -2209,18 +2359,15 @@
       <c r="M2" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="7">
         <v>1.2566650000000001E-6</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="7">
         <v>64100000</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="4">
         <v>0.3</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A3" s="4">
@@ -2259,18 +2406,15 @@
       <c r="M3" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <v>1.25664E-6</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="7">
         <v>58000000</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="4">
         <v>0.3</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A4" s="4">
@@ -2309,18 +2453,15 @@
       <c r="M4" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <v>6.3E-3</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <v>11200000</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="4">
         <v>0.3</v>
       </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A5" s="4">
@@ -2359,9 +2500,6 @@
       <c r="N5" s="4">
         <v>100</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A6" s="4">
@@ -2400,7 +2538,7 @@
     </row>
     <row r="7" spans="1:20" ht="171" x14ac:dyDescent="0.85">
       <c r="A7" s="4">
-        <v>152</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>126</v>
@@ -2420,25 +2558,25 @@
       <c r="G7" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>487</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>30000000</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="7">
         <v>1000000000</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="171" x14ac:dyDescent="0.85">
       <c r="A8" s="4">
-        <v>153</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>126</v>
@@ -2458,25 +2596,25 @@
       <c r="G8" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="8" t="s">
         <v>489</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="8" t="s">
         <v>490</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="7">
         <v>30000000</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="7">
         <v>1000000000</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A9" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -2508,13 +2646,10 @@
       <c r="M9" s="4">
         <v>10</v>
       </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A10" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>10</v>
@@ -2552,7 +2687,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A11" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>10</v>
@@ -2593,7 +2728,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A12" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>10</v>
@@ -2631,13 +2766,10 @@
       <c r="N12" s="4">
         <v>50</v>
       </c>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A13" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>10</v>
@@ -2672,13 +2804,10 @@
       <c r="N13" s="4">
         <v>50</v>
       </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A14" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>10</v>
@@ -2713,13 +2842,10 @@
       <c r="N14" s="4">
         <v>50</v>
       </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A15" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>10</v>
@@ -2754,13 +2880,10 @@
       <c r="N15" s="4">
         <v>50</v>
       </c>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.85">
       <c r="A16" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>10</v>
@@ -2795,13 +2918,10 @@
       <c r="N16" s="4">
         <v>50</v>
       </c>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A17" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>10</v>
@@ -2836,13 +2956,10 @@
       <c r="N17" s="4">
         <v>50</v>
       </c>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A18" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>10</v>
@@ -2877,13 +2994,10 @@
       <c r="N18" s="4">
         <v>50</v>
       </c>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A19" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>10</v>
@@ -2918,13 +3032,10 @@
       <c r="N19" s="4">
         <v>50</v>
       </c>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A20" s="4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>10</v>
@@ -2959,13 +3070,10 @@
       <c r="N20" s="4">
         <v>50</v>
       </c>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A21" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>10</v>
@@ -3000,13 +3108,10 @@
       <c r="M21" s="4">
         <v>120</v>
       </c>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A22" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>10</v>
@@ -3042,9 +3147,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A23" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>10</v>
@@ -3080,9 +3185,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A24" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>10</v>
@@ -3117,13 +3222,10 @@
       <c r="N24" s="4">
         <v>50</v>
       </c>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A25" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>10</v>
@@ -3161,13 +3263,10 @@
       <c r="N25" s="4">
         <v>50</v>
       </c>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A26" s="4">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>10</v>
@@ -3206,9 +3305,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A27" s="4">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>10</v>
@@ -3244,9 +3343,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A28" s="4">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>10</v>
@@ -3285,9 +3384,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A29" s="4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>10</v>
@@ -3326,9 +3425,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A30" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>10</v>
@@ -3367,9 +3466,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A31" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>102</v>
@@ -3404,13 +3503,10 @@
       <c r="N31" s="4">
         <v>100</v>
       </c>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A32" s="4">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>102</v>
@@ -3445,13 +3541,10 @@
       <c r="M32" s="4">
         <v>100</v>
       </c>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A33" s="4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>102</v>
@@ -3492,12 +3585,10 @@
       <c r="O33" s="4">
         <v>0.01</v>
       </c>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A34" s="4">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>102</v>
@@ -3529,13 +3620,10 @@
       <c r="M34" s="4">
         <v>100</v>
       </c>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A35" s="4">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>102</v>
@@ -3573,12 +3661,10 @@
       <c r="O35" s="4">
         <v>0.01</v>
       </c>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A36" s="4">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>379</v>
@@ -3611,9 +3697,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="228" x14ac:dyDescent="0.85">
+    <row r="37" spans="1:15" ht="228" x14ac:dyDescent="0.85">
       <c r="A37" s="4">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>126</v>
@@ -3633,25 +3719,25 @@
       <c r="G37" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="8" t="s">
         <v>474</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L37" s="8">
+      <c r="L37" s="7">
         <v>1000000</v>
       </c>
-      <c r="M37" s="8">
+      <c r="M37" s="7">
         <v>1000000000</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="228" x14ac:dyDescent="0.85">
+    <row r="38" spans="1:15" ht="228" x14ac:dyDescent="0.85">
       <c r="A38" s="4">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>126</v>
@@ -3671,25 +3757,25 @@
       <c r="G38" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="8" t="s">
         <v>473</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L38" s="8">
+      <c r="L38" s="7">
         <v>1000000</v>
       </c>
-      <c r="M38" s="8">
+      <c r="M38" s="7">
         <v>1000000000</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="171" x14ac:dyDescent="0.85">
+    <row r="39" spans="1:15" ht="171" x14ac:dyDescent="0.85">
       <c r="A39" s="4">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>126</v>
@@ -3709,25 +3795,25 @@
       <c r="G39" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I39" s="10" t="s">
+      <c r="I39" s="8" t="s">
         <v>477</v>
       </c>
-      <c r="J39" s="10" t="s">
+      <c r="J39" s="8" t="s">
         <v>478</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L39" s="8">
+      <c r="L39" s="7">
         <v>100000</v>
       </c>
-      <c r="M39" s="8">
+      <c r="M39" s="7">
         <v>50000000</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="171" x14ac:dyDescent="0.85">
+    <row r="40" spans="1:15" ht="171" x14ac:dyDescent="0.85">
       <c r="A40" s="4">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>126</v>
@@ -3747,25 +3833,25 @@
       <c r="G40" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I40" s="10" t="s">
+      <c r="I40" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="J40" s="10" t="s">
+      <c r="J40" s="8" t="s">
         <v>475</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L40" s="8">
+      <c r="L40" s="7">
         <v>100000</v>
       </c>
-      <c r="M40" s="8">
+      <c r="M40" s="7">
         <v>50000000</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="228" x14ac:dyDescent="0.85">
+    <row r="41" spans="1:15" ht="228" x14ac:dyDescent="0.85">
       <c r="A41" s="4">
-        <v>151</v>
+        <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>126</v>
@@ -3785,25 +3871,25 @@
       <c r="G41" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="I41" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J41" s="8" t="s">
         <v>484</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L41" s="8">
+      <c r="L41" s="7">
         <v>150000</v>
       </c>
-      <c r="M41" s="8">
+      <c r="M41" s="7">
         <v>30000000</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="228" x14ac:dyDescent="0.85">
+    <row r="42" spans="1:15" ht="228" x14ac:dyDescent="0.85">
       <c r="A42" s="4">
-        <v>150</v>
+        <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>126</v>
@@ -3823,25 +3909,25 @@
       <c r="G42" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I42" s="10" t="s">
+      <c r="I42" s="8" t="s">
         <v>480</v>
       </c>
-      <c r="J42" s="10" t="s">
+      <c r="J42" s="8" t="s">
         <v>483</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L42" s="8">
+      <c r="L42" s="7">
         <v>150000</v>
       </c>
-      <c r="M42" s="8">
+      <c r="M42" s="7">
         <v>30000000</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A43" s="4">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>102</v>
@@ -3876,13 +3962,10 @@
       <c r="M43" s="4">
         <v>50</v>
       </c>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A44" s="4">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>32</v>
@@ -3915,9 +3998,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A45" s="4">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>102</v>
@@ -3949,13 +4032,10 @@
       <c r="M45" s="4">
         <v>100</v>
       </c>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A46" s="4">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>286</v>
@@ -3988,9 +4068,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A47" s="4">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>286</v>
@@ -4023,9 +4103,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A48" s="4">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>286</v>
@@ -4058,9 +4138,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A49" s="4">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>286</v>
@@ -4093,9 +4173,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A50" s="4">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>286</v>
@@ -4128,9 +4208,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A51" s="4">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>286</v>
@@ -4163,9 +4243,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A52" s="4">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>286</v>
@@ -4198,9 +4278,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A53" s="4">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>286</v>
@@ -4233,9 +4313,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A54" s="4">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>286</v>
@@ -4268,9 +4348,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A55" s="4">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>286</v>
@@ -4303,9 +4383,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A56" s="4">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>286</v>
@@ -4338,9 +4418,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A57" s="4">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>286</v>
@@ -4373,9 +4453,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A58" s="4">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>286</v>
@@ -4408,9 +4488,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A59" s="4">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>286</v>
@@ -4443,9 +4523,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A60" s="4">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>286</v>
@@ -4478,9 +4558,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A61" s="4">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>286</v>
@@ -4512,13 +4592,10 @@
       <c r="M61" s="4">
         <v>10000</v>
       </c>
-      <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A62" s="4">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>286</v>
@@ -4550,13 +4627,10 @@
       <c r="M62" s="4">
         <v>10000</v>
       </c>
-      <c r="R62" s="4"/>
-      <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A63" s="4">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>286</v>
@@ -4588,13 +4662,10 @@
       <c r="M63" s="4">
         <v>10000</v>
       </c>
-      <c r="R63" s="4"/>
-      <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A64" s="4">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>286</v>
@@ -4627,9 +4698,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A65" s="4">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>286</v>
@@ -4661,13 +4732,10 @@
       <c r="M65" s="4">
         <v>10000</v>
       </c>
-      <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A66" s="4">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>286</v>
@@ -4699,16 +4767,10 @@
       <c r="M66" s="4">
         <v>10</v>
       </c>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
-      <c r="Q66" s="4"/>
-      <c r="R66" s="4"/>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A67" s="4">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>286</v>
@@ -4740,13 +4802,10 @@
       <c r="M67" s="4">
         <v>10000</v>
       </c>
-      <c r="R67" s="4"/>
-      <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A68" s="4">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>286</v>
@@ -4779,9 +4838,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A69" s="4">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>286</v>
@@ -4814,9 +4873,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A70" s="4">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>286</v>
@@ -4849,9 +4908,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A71" s="4">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>286</v>
@@ -4884,9 +4943,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A72" s="4">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>286</v>
@@ -4919,9 +4978,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A73" s="4">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>286</v>
@@ -4954,9 +5013,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A74" s="4">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>286</v>
@@ -4989,9 +5048,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A75" s="4">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>286</v>
@@ -5024,9 +5083,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A76" s="4">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>286</v>
@@ -5058,13 +5117,10 @@
       <c r="M76" s="4">
         <v>100</v>
       </c>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
-      <c r="Q76" s="4"/>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A77" s="4">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>286</v>
@@ -5097,9 +5153,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A78" s="4">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>286</v>
@@ -5132,9 +5188,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A79" s="4">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>286</v>
@@ -5167,9 +5223,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.85">
       <c r="A80" s="4">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>286</v>
@@ -5202,9 +5258,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A81" s="4">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>286</v>
@@ -5236,13 +5292,10 @@
       <c r="M81" s="4">
         <v>10000</v>
       </c>
-      <c r="R81" s="4"/>
-      <c r="S81" s="4"/>
-      <c r="T81" s="4"/>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A82" s="4">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>102</v>
@@ -5274,16 +5327,10 @@
       <c r="M82" s="4">
         <v>20</v>
       </c>
-      <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
-      <c r="Q82" s="4"/>
-      <c r="R82" s="4"/>
-      <c r="S82" s="4"/>
-      <c r="T82" s="4"/>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A83" s="4">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>102</v>
@@ -5315,13 +5362,10 @@
       <c r="M83" s="4">
         <v>100</v>
       </c>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
-      <c r="Q83" s="4"/>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A84" s="4">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>102</v>
@@ -5356,19 +5400,19 @@
       <c r="M84" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N84" s="8">
+      <c r="N84" s="7">
         <v>1.2566650000000001E-6</v>
       </c>
-      <c r="O84" s="9">
+      <c r="O84" s="7">
         <v>64100000</v>
       </c>
-      <c r="P84" s="7">
+      <c r="P84" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A85" s="4">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>102</v>
@@ -5403,19 +5447,19 @@
       <c r="M85" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N85" s="8">
+      <c r="N85" s="7">
         <v>1.25664E-6</v>
       </c>
-      <c r="O85" s="9">
+      <c r="O85" s="7">
         <v>58000000</v>
       </c>
-      <c r="P85" s="7">
+      <c r="P85" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A86" s="4">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>102</v>
@@ -5450,19 +5494,19 @@
       <c r="M86" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N86" s="8">
+      <c r="N86" s="7">
         <v>6.3E-3</v>
       </c>
-      <c r="O86" s="9">
+      <c r="O86" s="7">
         <v>11200000</v>
       </c>
-      <c r="P86" s="7">
+      <c r="P86" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A87" s="4">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>460</v>
@@ -5494,13 +5538,10 @@
       <c r="M87" s="4">
         <v>5</v>
       </c>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
-      <c r="Q87" s="4"/>
-    </row>
-    <row r="88" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    </row>
+    <row r="88" spans="1:16" ht="199.5" x14ac:dyDescent="0.85">
       <c r="A88" s="4">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>102</v>
@@ -5520,10 +5561,10 @@
       <c r="G88" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I88" s="10" t="s">
+      <c r="I88" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="J88" s="10" t="s">
+      <c r="J88" s="8" t="s">
         <v>443</v>
       </c>
       <c r="K88" s="4" t="s">
@@ -5545,9 +5586,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="89" spans="1:16" ht="199.5" x14ac:dyDescent="0.85">
       <c r="A89" s="4">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>102</v>
@@ -5567,10 +5608,10 @@
       <c r="G89" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I89" s="10" t="s">
+      <c r="I89" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="J89" s="10" t="s">
+      <c r="J89" s="8" t="s">
         <v>443</v>
       </c>
       <c r="K89" s="4" t="s">
@@ -5592,9 +5633,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="90" spans="1:16" ht="199.5" x14ac:dyDescent="0.85">
       <c r="A90" s="4">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>102</v>
@@ -5614,10 +5655,10 @@
       <c r="G90" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I90" s="10" t="s">
+      <c r="I90" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="J90" s="10" t="s">
+      <c r="J90" s="8" t="s">
         <v>443</v>
       </c>
       <c r="K90" s="4" t="s">
@@ -5639,9 +5680,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="91" spans="1:16" ht="199.5" x14ac:dyDescent="0.85">
       <c r="A91" s="4">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>102</v>
@@ -5661,10 +5702,10 @@
       <c r="G91" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I91" s="10" t="s">
+      <c r="I91" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="J91" s="10" t="s">
+      <c r="J91" s="8" t="s">
         <v>438</v>
       </c>
       <c r="K91" s="4" t="s">
@@ -5686,9 +5727,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="92" spans="1:16" ht="199.5" x14ac:dyDescent="0.85">
       <c r="A92" s="4">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>102</v>
@@ -5708,10 +5749,10 @@
       <c r="G92" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I92" s="10" t="s">
+      <c r="I92" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="J92" s="10" t="s">
+      <c r="J92" s="8" t="s">
         <v>467</v>
       </c>
       <c r="K92" s="4" t="s">
@@ -5733,9 +5774,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="199.5" x14ac:dyDescent="0.85">
+    <row r="93" spans="1:16" ht="199.5" x14ac:dyDescent="0.85">
       <c r="A93" s="4">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>102</v>
@@ -5755,10 +5796,10 @@
       <c r="G93" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I93" s="10" t="s">
+      <c r="I93" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="J93" s="10" t="s">
+      <c r="J93" s="8" t="s">
         <v>467</v>
       </c>
       <c r="K93" s="4" t="s">
@@ -5780,9 +5821,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A94" s="4">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>102</v>
@@ -5817,13 +5858,10 @@
       <c r="M94" s="4">
         <v>10</v>
       </c>
-      <c r="O94" s="4"/>
-      <c r="P94" s="4"/>
-      <c r="Q94" s="4"/>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.85">
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A95" s="4">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>390</v>
@@ -5862,9 +5900,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.85">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.85">
       <c r="A96" s="4">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>32</v>
@@ -5897,9 +5935,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A97" s="4">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>102</v>
@@ -5937,16 +5975,16 @@
       <c r="M97" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N97" s="8">
+      <c r="N97" s="7">
         <v>1.2566650000000001E-6</v>
       </c>
-      <c r="O97" s="9">
+      <c r="O97" s="7">
         <v>64100000</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A98" s="4">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>102</v>
@@ -5984,16 +6022,16 @@
       <c r="M98" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N98" s="8">
+      <c r="N98" s="7">
         <v>1.25664E-6</v>
       </c>
-      <c r="O98" s="9">
+      <c r="O98" s="7">
         <v>58000000</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A99" s="4">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>102</v>
@@ -6031,16 +6069,16 @@
       <c r="M99" s="4">
         <v>20000000000</v>
       </c>
-      <c r="N99" s="8">
+      <c r="N99" s="7">
         <v>6.3E-3</v>
       </c>
-      <c r="O99" s="9">
+      <c r="O99" s="7">
         <v>11200000</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A100" s="4">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>102</v>
@@ -6078,12 +6116,10 @@
       <c r="O100" s="4">
         <v>0.1</v>
       </c>
-      <c r="P100" s="4"/>
-      <c r="Q100" s="4"/>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A101" s="4">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>102</v>
@@ -6115,13 +6151,10 @@
       <c r="M101" s="4">
         <v>100</v>
       </c>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
-      <c r="Q101" s="4"/>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A102" s="4">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>10</v>
@@ -6154,9 +6187,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A103" s="4">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>10</v>
@@ -6192,9 +6225,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A104" s="4">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>10</v>
@@ -6230,9 +6263,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A105" s="4">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>10</v>
@@ -6265,9 +6298,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A106" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>10</v>
@@ -6300,9 +6333,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A107" s="4">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>10</v>
@@ -6337,13 +6370,10 @@
       <c r="M107" s="4">
         <v>50</v>
       </c>
-      <c r="O107" s="4"/>
-      <c r="P107" s="4"/>
-      <c r="Q107" s="4"/>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A108" s="4">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>10</v>
@@ -6378,13 +6408,10 @@
       <c r="N108" s="4">
         <v>50</v>
       </c>
-      <c r="O108" s="4"/>
-      <c r="P108" s="4"/>
-      <c r="Q108" s="4"/>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A109" s="4">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>10</v>
@@ -6417,9 +6444,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A110" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>10</v>
@@ -6455,9 +6482,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A111" s="4">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>10</v>
@@ -6493,9 +6520,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.85">
       <c r="A112" s="4">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>10</v>
@@ -6531,9 +6558,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A113" s="4">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>10</v>
@@ -6569,9 +6596,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A114" s="4">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>10</v>
@@ -6610,9 +6637,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A115" s="4">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>10</v>
@@ -6648,9 +6675,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A116" s="4">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>10</v>
@@ -6686,9 +6713,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A117" s="4">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>10</v>
@@ -6727,9 +6754,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A118" s="4">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>10</v>
@@ -6765,9 +6792,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A119" s="4">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>10</v>
@@ -6803,9 +6830,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A120" s="4">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>10</v>
@@ -6841,9 +6868,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A121" s="4">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>10</v>
@@ -6885,9 +6912,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A122" s="4">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>10</v>
@@ -6920,9 +6947,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A123" s="4">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>10</v>
@@ -6955,9 +6982,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A124" s="4">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>10</v>
@@ -6990,9 +7017,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A125" s="4">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>10</v>
@@ -7030,13 +7057,10 @@
       <c r="N125" s="4">
         <v>50</v>
       </c>
-      <c r="O125" s="4"/>
-      <c r="P125" s="4"/>
-      <c r="Q125" s="4"/>
-    </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A126" s="4">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>10</v>
@@ -7074,13 +7098,10 @@
       <c r="N126" s="4">
         <v>50</v>
       </c>
-      <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
-      <c r="Q126" s="4"/>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.85">
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A127" s="4">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>10</v>
@@ -7113,9 +7134,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.85">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A128" s="4">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>10</v>
@@ -7150,7 +7171,7 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A129" s="4">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>10</v>
@@ -7185,7 +7206,7 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A130" s="4">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>10</v>
@@ -7223,7 +7244,7 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A131" s="4">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>10</v>
@@ -7261,7 +7282,7 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A132" s="4">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>10</v>
@@ -7299,7 +7320,7 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A133" s="4">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>10</v>
@@ -7334,13 +7355,10 @@
       <c r="N133" s="4">
         <v>50</v>
       </c>
-      <c r="O133" s="4"/>
-      <c r="P133" s="4"/>
-      <c r="Q133" s="4"/>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A134" s="4">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>10</v>
@@ -7375,7 +7393,7 @@
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A135" s="4">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>10</v>
@@ -7407,13 +7425,10 @@
       <c r="M135" s="4">
         <v>100</v>
       </c>
-      <c r="O135" s="4"/>
-      <c r="P135" s="4"/>
-      <c r="Q135" s="4"/>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A136" s="4">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>10</v>
@@ -7451,7 +7466,7 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A137" s="4">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>10</v>
@@ -7489,7 +7504,7 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A138" s="4">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>10</v>
@@ -7524,7 +7539,7 @@
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A139" s="4">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>10</v>
@@ -7562,7 +7577,7 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A140" s="4">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>10</v>
@@ -7600,7 +7615,7 @@
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A141" s="4">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>10</v>
@@ -7635,7 +7650,7 @@
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A142" s="4">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>10</v>
@@ -7673,7 +7688,7 @@
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A143" s="4">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>10</v>
@@ -7714,7 +7729,7 @@
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A144" s="4">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>10</v>
@@ -7752,13 +7767,13 @@
       <c r="N144" s="4">
         <v>50</v>
       </c>
-      <c r="R144" s="8">
+      <c r="R144" s="7">
         <v>11200000</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A145" s="4">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>10</v>
@@ -7796,13 +7811,13 @@
       <c r="N145" s="4">
         <v>50</v>
       </c>
-      <c r="R145" s="8">
+      <c r="R145" s="7">
         <v>11200000</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A146" s="4">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>10</v>
@@ -7843,7 +7858,7 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A147" s="4">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>10</v>
@@ -7881,7 +7896,7 @@
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A148" s="4">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>10</v>
@@ -7922,7 +7937,7 @@
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A149" s="4">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>10</v>
@@ -7963,7 +7978,7 @@
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A150" s="4">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>10</v>
@@ -8001,13 +8016,10 @@
       <c r="N150" s="4">
         <v>50</v>
       </c>
-      <c r="O150" s="4"/>
-      <c r="P150" s="4"/>
-      <c r="Q150" s="4"/>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A151" s="4">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>10</v>
@@ -8045,7 +8057,7 @@
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A152" s="4">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>10</v>
@@ -8083,7 +8095,7 @@
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A153" s="4">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>32</v>
@@ -8121,7 +8133,7 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.85">
       <c r="A154" s="4">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>32</v>
@@ -8158,6 +8170,9 @@
       </c>
     </row>
     <row r="155" spans="1:18" ht="199.5" x14ac:dyDescent="0.85">
+      <c r="A155" s="4">
+        <v>154</v>
+      </c>
       <c r="B155" s="4" t="s">
         <v>126</v>
       </c>
@@ -8176,23 +8191,26 @@
       <c r="G155" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I155" s="10" t="s">
+      <c r="I155" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="J155" s="10" t="s">
+      <c r="J155" s="8" t="s">
         <v>493</v>
       </c>
       <c r="K155" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L155" s="8">
+      <c r="L155" s="7">
         <v>30000000</v>
       </c>
-      <c r="M155" s="8">
+      <c r="M155" s="7">
         <v>10000000000</v>
       </c>
     </row>
     <row r="156" spans="1:18" ht="199.5" x14ac:dyDescent="0.85">
+      <c r="A156" s="4">
+        <v>155</v>
+      </c>
       <c r="B156" s="4" t="s">
         <v>126</v>
       </c>
@@ -8211,24 +8229,479 @@
       <c r="G156" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I156" s="10" t="s">
+      <c r="I156" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="J156" s="10" t="s">
+      <c r="J156" s="8" t="s">
         <v>496</v>
       </c>
       <c r="K156" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L156" s="8">
+      <c r="L156" s="7">
         <v>30000000</v>
       </c>
-      <c r="M156" s="8">
+      <c r="M156" s="7">
         <v>10000000000</v>
       </c>
     </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.85">
+      <c r="A157" s="4">
+        <v>156</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F157" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I157" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="J157" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="K157" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="L157" s="4">
+        <v>0</v>
+      </c>
+      <c r="M157" s="4">
+        <v>100</v>
+      </c>
+      <c r="N157" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.85">
+      <c r="A158" s="4">
+        <v>157</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="F158" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="H158" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I158" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="J158" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="K158" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L158" s="4">
+        <v>-120</v>
+      </c>
+      <c r="M158" s="4">
+        <v>50</v>
+      </c>
+      <c r="N158" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" ht="199.5" x14ac:dyDescent="0.85">
+      <c r="A159" s="4">
+        <v>158</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="F159" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="I159" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="J159" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="K159" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="L159" s="4">
+        <v>1</v>
+      </c>
+      <c r="M159" s="4">
+        <v>5</v>
+      </c>
+      <c r="N159" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="O159" s="7">
+        <v>0.63500000000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" ht="199.5" x14ac:dyDescent="0.85">
+      <c r="A160" s="4">
+        <v>159</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="F160" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="I160" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="J160" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="K160" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="L160" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="M160" s="4">
+        <v>10</v>
+      </c>
+      <c r="N160" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O160" s="7">
+        <v>0.63500000000000001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" ht="199.5" x14ac:dyDescent="0.85">
+      <c r="A161" s="4">
+        <v>160</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="I161" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="J161" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="K161" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="L161" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="M161" s="4">
+        <v>1</v>
+      </c>
+      <c r="N161" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O161" s="7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" ht="114" x14ac:dyDescent="0.85">
+      <c r="A162" s="4">
+        <v>161</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="F162" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="G162" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I162" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="J162" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="K162" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="L162" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="M162" s="4">
+        <v>1</v>
+      </c>
+      <c r="N162" s="7">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="O162" s="7"/>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="A163" s="4">
+        <v>162</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C163" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="F163" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I163" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="J163" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="K163" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="L163" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="M163" s="4">
+        <v>1000</v>
+      </c>
+      <c r="N163" s="7"/>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="A164" s="4">
+        <v>163</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E164" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="F164" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I164" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="J164" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="K164" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="L164" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="M164" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="A165" s="4">
+        <v>164</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="F165" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="I165" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="J165" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="K165" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="L165" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="M165" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="A166" s="4">
+        <v>165</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="F166" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="I166" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="J166" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="K166" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="L166" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="M166" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="A167" s="4">
+        <v>166</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="E167" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="F167" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="I167" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="J167" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="K167" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="L167" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="M167" s="4">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="A168" s="4">
+        <v>167</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="E168" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="F168" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I168" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="J168" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="K168" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="L168" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="M168" s="4">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q156" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:Q157" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q154">
       <sortCondition ref="E1:E154"/>
     </sortState>

</xml_diff>